<commit_message>
variable updates; added '-' for empty cells
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ8_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ8_PH2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="205">
   <si>
     <t>Probe</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Desert Triage Performance</t>
   </si>
   <si>
-    <t>Desert Tagging performance</t>
-  </si>
-  <si>
     <t>Desert Hemorrhage control</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>Urban Triage Performance</t>
   </si>
   <si>
-    <t>Urban Tagging performance</t>
-  </si>
-  <si>
     <t>Urban Hemorrhage control</t>
   </si>
   <si>
@@ -679,9 +673,6 @@
   </si>
   <si>
     <t>% correct treatments applied</t>
-  </si>
-  <si>
-    <t>% correct tags applied</t>
   </si>
   <si>
     <t>Yes (1) if all hemorrhage control actions takens; otherwise no</t>
@@ -821,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -843,9 +834,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1149,7 +1137,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:EO4"/>
+  <dimension ref="A1:EM4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1166,12 +1154,12 @@
     <col min="9" max="9" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
@@ -1182,17 +1170,17 @@
     <col min="25" max="25" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="26" max="26" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="27" max="27" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="30" max="30" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="31" max="31" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="32" max="32" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="35" max="35" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="36" max="36" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="39" max="39" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="40" max="40" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="41" max="41" style="6" width="13.005" customWidth="1" bestFit="1"/>
@@ -1298,8 +1286,6 @@
     <col min="141" max="141" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="142" max="142" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="143" max="143" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="144" max="144" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="145" max="145" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="46.5" customFormat="1" s="7">
@@ -1732,1320 +1718,1296 @@
       <c r="EM1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="EN1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="EO1" s="3" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33" customFormat="1" s="7">
       <c r="A2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BM2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BN2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BP2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BQ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BR2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BS2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BT2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BU2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BV2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BW2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BX2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BY2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BZ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CD2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CM2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CN2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CP2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CQ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CR2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CS2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CT2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CU2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CV2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CW2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CX2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CY2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CZ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DD2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DM2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DN2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DP2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DQ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DR2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DS2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DT2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DU2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DV2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DW2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DX2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DY2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DZ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ED2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EM2" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="EN2" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="EO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="154.5" customFormat="1" s="7">
       <c r="A3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="N3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="T3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="V3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="W3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AG3" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AM3" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AN3" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AO3" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AP3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AR3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AS3" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AV3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AP3" s="3" t="s">
+      <c r="AW3" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="AQ3" s="3" t="s">
+      <c r="AX3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AR3" s="3" t="s">
+      <c r="AY3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AZ3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AT3" s="3" t="s">
+      <c r="BA3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AU3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="AV3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="AX3" s="3" t="s">
+      <c r="BB3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BC3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BD3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BE3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AY3" s="3" t="s">
+      <c r="BF3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="BG3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BA3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BB3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BC3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="BD3" s="3" t="s">
+      <c r="BH3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BI3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BJ3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BK3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="BE3" s="3" t="s">
+      <c r="BL3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BF3" s="3" t="s">
+      <c r="BM3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BG3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BH3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BI3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="BJ3" s="3" t="s">
+      <c r="BN3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BO3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BP3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BQ3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="BK3" s="3" t="s">
+      <c r="BR3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BL3" s="3" t="s">
+      <c r="BS3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BM3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BN3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BO3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="BP3" s="3" t="s">
+      <c r="BT3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BU3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BV3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BW3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="BQ3" s="3" t="s">
+      <c r="BX3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BR3" s="3" t="s">
+      <c r="BY3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BS3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BT3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BU3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="BV3" s="3" t="s">
+      <c r="BZ3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CA3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CB3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CC3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="BW3" s="3" t="s">
+      <c r="CD3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BX3" s="3" t="s">
+      <c r="CE3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BY3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BZ3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CA3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CB3" s="3" t="s">
+      <c r="CF3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CG3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CH3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CI3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="CC3" s="3" t="s">
+      <c r="CJ3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="CD3" s="3" t="s">
+      <c r="CK3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="CE3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CF3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CG3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CH3" s="3" t="s">
+      <c r="CL3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CM3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CN3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CO3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="CI3" s="3" t="s">
+      <c r="CP3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="CJ3" s="3" t="s">
+      <c r="CQ3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="CK3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CL3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CM3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CN3" s="3" t="s">
+      <c r="CR3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CS3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CT3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CU3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="CO3" s="3" t="s">
+      <c r="CV3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="CP3" s="3" t="s">
+      <c r="CW3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="CQ3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CR3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CS3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CT3" s="3" t="s">
+      <c r="CX3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CY3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CZ3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DA3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="CU3" s="3" t="s">
+      <c r="DB3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="CV3" s="3" t="s">
+      <c r="DC3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="CW3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CX3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CY3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CZ3" s="3" t="s">
+      <c r="DD3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DE3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DF3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DG3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DA3" s="3" t="s">
+      <c r="DH3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DB3" s="3" t="s">
+      <c r="DI3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="DC3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DD3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DE3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="DF3" s="3" t="s">
+      <c r="DJ3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DK3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DL3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DM3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DG3" s="3" t="s">
+      <c r="DN3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DH3" s="3" t="s">
+      <c r="DO3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="DI3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DJ3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DK3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="DL3" s="3" t="s">
+      <c r="DP3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DQ3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DR3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DS3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DM3" s="3" t="s">
+      <c r="DT3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DN3" s="3" t="s">
+      <c r="DU3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="DO3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DP3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DQ3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="DR3" s="3" t="s">
+      <c r="DV3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DW3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DX3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DY3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DS3" s="3" t="s">
+      <c r="DZ3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DT3" s="3" t="s">
+      <c r="EA3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="DU3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DV3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DW3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="DX3" s="3" t="s">
+      <c r="EB3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="EC3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="ED3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="EE3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DY3" s="3" t="s">
+      <c r="EF3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DZ3" s="3" t="s">
+      <c r="EG3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="EA3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="EB3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="EC3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="ED3" s="3" t="s">
+      <c r="EH3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="EI3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="EJ3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="EK3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="EE3" s="3" t="s">
+      <c r="EL3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="EF3" s="3" t="s">
+      <c r="EM3" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="EG3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="EH3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="EI3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="EJ3" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="EK3" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="EL3" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="EM3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="EN3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="EO3" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="100.5" customFormat="1" s="7">
       <c r="A4" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="S4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF4" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AK4" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="AO4" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="AA4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AU4" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="AV4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="AW4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AX4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="AY4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AZ4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BA4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BB4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BC4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="BD4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="BE4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="BF4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BG4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BH4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BI4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="BJ4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="BK4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="BL4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BM4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BN4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BO4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="BP4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="BQ4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="BR4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BS4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BT4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BU4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="BV4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="BW4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="BX4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BY4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BZ4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CA4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CB4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="CC4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CD4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="CE4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="CF4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CG4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CH4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="CI4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CJ4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="CK4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="CL4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CM4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CN4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="CO4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CP4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="CQ4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="CR4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CS4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CT4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="CU4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CV4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="CW4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="CX4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CY4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CZ4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="DA4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DB4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="DC4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="DD4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="DE4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="DF4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="DG4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DH4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="DI4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="DJ4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="DK4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="DL4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="DM4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DN4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="DO4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="DP4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="DQ4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="DR4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="DS4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DT4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="DU4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="DV4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="DW4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="DX4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="DY4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DZ4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="EA4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="EB4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="EC4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="ED4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="EE4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="EF4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="EG4" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="EH4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="EI4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="EJ4" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="EK4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="EL4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="EM4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="EN4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="EO4" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round to 2 decimals; updated time units in variables sheet
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ8_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ8_PH2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="204">
   <si>
     <t>Probe</t>
   </si>
@@ -672,7 +672,7 @@
     <t xml:space="preserve">Search vs. Stay probe based on whether the participant searched for new patients or stayed with current patients </t>
   </si>
   <si>
-    <t>% correct treatments applied</t>
+    <t>% correct treatments applied calculated as (correct tools applied) / (misses + total tools applied).</t>
   </si>
   <si>
     <t>Yes (1) if all hemorrhage control actions takens; otherwise no</t>
@@ -747,19 +747,16 @@
     <t>1 or 0</t>
   </si>
   <si>
-    <t>time (m)</t>
+    <t>time (s)</t>
   </si>
   <si>
     <t>number</t>
   </si>
   <si>
-    <t>time (ms)</t>
-  </si>
-  <si>
     <t>Yes/no</t>
   </si>
   <si>
-    <t>Time (ms)</t>
+    <t>Time (s)</t>
   </si>
   <si>
     <t>color of tag or N/A if none applied</t>
@@ -2662,10 +2659,10 @@
         <v>200</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AD4" s="3" t="s">
         <v>200</v>
@@ -2674,7 +2671,7 @@
         <v>194</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AG4" s="3" t="s">
         <v>200</v>
@@ -2689,10 +2686,10 @@
         <v>200</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AM4" s="3" t="s">
         <v>200</v>
@@ -2701,16 +2698,16 @@
         <v>194</v>
       </c>
       <c r="AO4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="AQ4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AS4" s="3" t="s">
         <v>200</v>
@@ -2719,16 +2716,16 @@
         <v>200</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AV4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AW4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="AX4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AY4" s="3" t="s">
         <v>200</v>
@@ -2737,16 +2734,16 @@
         <v>200</v>
       </c>
       <c r="BA4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BB4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BC4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="BD4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BE4" s="3" t="s">
         <v>200</v>
@@ -2755,16 +2752,16 @@
         <v>200</v>
       </c>
       <c r="BG4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BH4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BI4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="BJ4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BK4" s="3" t="s">
         <v>200</v>
@@ -2773,16 +2770,16 @@
         <v>200</v>
       </c>
       <c r="BM4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BN4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BO4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="BP4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BQ4" s="3" t="s">
         <v>200</v>
@@ -2791,16 +2788,16 @@
         <v>200</v>
       </c>
       <c r="BS4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BT4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BU4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="BV4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BW4" s="3" t="s">
         <v>200</v>
@@ -2809,16 +2806,16 @@
         <v>200</v>
       </c>
       <c r="BY4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BZ4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CA4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="CB4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="CC4" s="3" t="s">
         <v>200</v>
@@ -2827,16 +2824,16 @@
         <v>200</v>
       </c>
       <c r="CE4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CF4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CG4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="CH4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="CI4" s="3" t="s">
         <v>200</v>
@@ -2845,16 +2842,16 @@
         <v>200</v>
       </c>
       <c r="CK4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CL4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CM4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="CN4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="CO4" s="3" t="s">
         <v>200</v>
@@ -2863,16 +2860,16 @@
         <v>200</v>
       </c>
       <c r="CQ4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CR4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CS4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="CT4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="CU4" s="3" t="s">
         <v>200</v>
@@ -2881,16 +2878,16 @@
         <v>200</v>
       </c>
       <c r="CW4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CX4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CY4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="CZ4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DA4" s="3" t="s">
         <v>200</v>
@@ -2899,16 +2896,16 @@
         <v>200</v>
       </c>
       <c r="DC4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="DD4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DE4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="DF4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DG4" s="3" t="s">
         <v>200</v>
@@ -2917,16 +2914,16 @@
         <v>200</v>
       </c>
       <c r="DI4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="DJ4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DK4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="DL4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DM4" s="3" t="s">
         <v>200</v>
@@ -2935,16 +2932,16 @@
         <v>200</v>
       </c>
       <c r="DO4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="DP4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DQ4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="DR4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DS4" s="3" t="s">
         <v>200</v>
@@ -2953,16 +2950,16 @@
         <v>200</v>
       </c>
       <c r="DU4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="DV4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DW4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="DX4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="DY4" s="3" t="s">
         <v>200</v>
@@ -2971,16 +2968,16 @@
         <v>200</v>
       </c>
       <c r="EA4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="EB4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="EC4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="ED4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="EE4" s="3" t="s">
         <v>200</v>
@@ -2989,16 +2986,16 @@
         <v>200</v>
       </c>
       <c r="EG4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="EH4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="EI4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="EJ4" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="EK4" s="3" t="s">
         <v>200</v>
@@ -3007,7 +3004,7 @@
         <v>200</v>
       </c>
       <c r="EM4" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RQ8 variable updates; added '-' for empty cells (#325)
* variable updates; added '-' for empty cells

* round to 2 decimals; updated time units in variables sheet
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ8_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ8_PH2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="204">
   <si>
     <t>Probe</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Desert Triage Performance</t>
   </si>
   <si>
-    <t>Desert Tagging performance</t>
-  </si>
-  <si>
     <t>Desert Hemorrhage control</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>Urban Triage Performance</t>
   </si>
   <si>
-    <t>Urban Tagging performance</t>
-  </si>
-  <si>
     <t>Urban Hemorrhage control</t>
   </si>
   <si>
@@ -678,10 +672,7 @@
     <t xml:space="preserve">Search vs. Stay probe based on whether the participant searched for new patients or stayed with current patients </t>
   </si>
   <si>
-    <t>% correct treatments applied</t>
-  </si>
-  <si>
-    <t>% correct tags applied</t>
+    <t>% correct treatments applied calculated as (correct tools applied) / (misses + total tools applied).</t>
   </si>
   <si>
     <t>Yes (1) if all hemorrhage control actions takens; otherwise no</t>
@@ -756,19 +747,16 @@
     <t>1 or 0</t>
   </si>
   <si>
-    <t>time (m)</t>
+    <t>time (s)</t>
   </si>
   <si>
     <t>number</t>
   </si>
   <si>
-    <t>time (ms)</t>
-  </si>
-  <si>
     <t>Yes/no</t>
   </si>
   <si>
-    <t>Time (ms)</t>
+    <t>Time (s)</t>
   </si>
   <si>
     <t>color of tag or N/A if none applied</t>
@@ -821,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -843,9 +831,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1149,7 +1134,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:EO4"/>
+  <dimension ref="A1:EM4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1166,12 +1151,12 @@
     <col min="9" max="9" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
@@ -1182,17 +1167,17 @@
     <col min="25" max="25" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="26" max="26" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="27" max="27" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="30" max="30" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="31" max="31" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="32" max="32" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="35" max="35" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="36" max="36" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="39" max="39" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="40" max="40" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="41" max="41" style="6" width="13.005" customWidth="1" bestFit="1"/>
@@ -1298,8 +1283,6 @@
     <col min="141" max="141" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="142" max="142" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="143" max="143" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="144" max="144" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="145" max="145" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="46.5" customFormat="1" s="7">
@@ -1732,1320 +1715,1296 @@
       <c r="EM1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="EN1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="EO1" s="3" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33" customFormat="1" s="7">
       <c r="A2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BM2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BN2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BP2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BQ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BR2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BS2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BT2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BU2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BV2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BW2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BX2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BY2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="BZ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CD2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CM2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CN2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CP2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CQ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CR2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CS2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CT2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CU2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CV2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CW2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CX2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CY2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="CZ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DD2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DM2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DN2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DP2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DQ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DR2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DS2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DT2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DU2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DV2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DW2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DX2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DY2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="DZ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EA2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EB2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EC2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="ED2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EE2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EF2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EG2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EH2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EI2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EJ2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EK2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EL2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="EM2" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="EN2" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="EO2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="154.5" customFormat="1" s="7">
       <c r="A3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="N3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="T3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="V3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="W3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AG3" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AM3" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AN3" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AO3" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AP3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AR3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AI3" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="AM3" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AS3" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AV3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AP3" s="3" t="s">
+      <c r="AW3" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="AQ3" s="3" t="s">
+      <c r="AX3" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AR3" s="3" t="s">
+      <c r="AY3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AZ3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AT3" s="3" t="s">
+      <c r="BA3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AU3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="AV3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="AX3" s="3" t="s">
+      <c r="BB3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BC3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BD3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BE3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AY3" s="3" t="s">
+      <c r="BF3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="BG3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BA3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BB3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BC3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="BD3" s="3" t="s">
+      <c r="BH3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BI3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BJ3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BK3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="BE3" s="3" t="s">
+      <c r="BL3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BF3" s="3" t="s">
+      <c r="BM3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BG3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BH3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BI3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="BJ3" s="3" t="s">
+      <c r="BN3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BO3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BP3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BQ3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="BK3" s="3" t="s">
+      <c r="BR3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BL3" s="3" t="s">
+      <c r="BS3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BM3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BN3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BO3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="BP3" s="3" t="s">
+      <c r="BT3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BU3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BV3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="BW3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="BQ3" s="3" t="s">
+      <c r="BX3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BR3" s="3" t="s">
+      <c r="BY3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BS3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BT3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BU3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="BV3" s="3" t="s">
+      <c r="BZ3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CA3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CB3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CC3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="BW3" s="3" t="s">
+      <c r="CD3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="BX3" s="3" t="s">
+      <c r="CE3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="BY3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="BZ3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CA3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CB3" s="3" t="s">
+      <c r="CF3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CG3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CH3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CI3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="CC3" s="3" t="s">
+      <c r="CJ3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="CD3" s="3" t="s">
+      <c r="CK3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="CE3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CF3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CG3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CH3" s="3" t="s">
+      <c r="CL3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CM3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CN3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CO3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="CI3" s="3" t="s">
+      <c r="CP3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="CJ3" s="3" t="s">
+      <c r="CQ3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="CK3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CL3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CM3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CN3" s="3" t="s">
+      <c r="CR3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CS3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CT3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="CU3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="CO3" s="3" t="s">
+      <c r="CV3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="CP3" s="3" t="s">
+      <c r="CW3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="CQ3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CR3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CS3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CT3" s="3" t="s">
+      <c r="CX3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="CY3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="CZ3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DA3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="CU3" s="3" t="s">
+      <c r="DB3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="CV3" s="3" t="s">
+      <c r="DC3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="CW3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CX3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CY3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="CZ3" s="3" t="s">
+      <c r="DD3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DE3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DF3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DG3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DA3" s="3" t="s">
+      <c r="DH3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DB3" s="3" t="s">
+      <c r="DI3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="DC3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DD3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DE3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="DF3" s="3" t="s">
+      <c r="DJ3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DK3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DL3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DM3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DG3" s="3" t="s">
+      <c r="DN3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DH3" s="3" t="s">
+      <c r="DO3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="DI3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DJ3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DK3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="DL3" s="3" t="s">
+      <c r="DP3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DQ3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DR3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DS3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DM3" s="3" t="s">
+      <c r="DT3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DN3" s="3" t="s">
+      <c r="DU3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="DO3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DP3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DQ3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="DR3" s="3" t="s">
+      <c r="DV3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="DW3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="DX3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="DY3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DS3" s="3" t="s">
+      <c r="DZ3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DT3" s="3" t="s">
+      <c r="EA3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="DU3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DV3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DW3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="DX3" s="3" t="s">
+      <c r="EB3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="EC3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="ED3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="EE3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="DY3" s="3" t="s">
+      <c r="EF3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="DZ3" s="3" t="s">
+      <c r="EG3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="EA3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="EB3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="EC3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="ED3" s="3" t="s">
+      <c r="EH3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="EI3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="EJ3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="EK3" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="EE3" s="3" t="s">
+      <c r="EL3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="EF3" s="3" t="s">
+      <c r="EM3" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="EG3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="EH3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="EI3" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="EJ3" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="EK3" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="EL3" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="EM3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="EN3" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="EO3" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="100.5" customFormat="1" s="7">
       <c r="A4" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="S4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="X4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AK4" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AM4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="V4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="AU4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="AV4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AW4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AX4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="AY4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AZ4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BA4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BB4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BC4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="BD4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="BE4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="BF4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BG4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BH4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BI4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="BJ4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="BK4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="BL4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BM4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BN4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BO4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="BP4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="BQ4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="BR4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BS4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BT4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BU4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="BV4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="BW4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="BX4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="BY4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="BZ4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CA4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CB4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="CC4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CD4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="CE4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CF4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CG4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CH4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="CI4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CJ4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="CK4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CL4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CM4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CN4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="CO4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CP4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="CQ4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CR4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CS4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CT4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="CU4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CV4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="CW4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="CX4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CY4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="CZ4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="DA4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DB4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="DC4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="DD4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DE4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="DF4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="DG4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DH4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="DI4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="DJ4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DK4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="DL4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="DM4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DN4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="DO4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="DP4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DQ4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="DR4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="DS4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DT4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="DU4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="DV4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DW4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="DX4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="DY4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DZ4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="EA4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="EB4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="EC4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="ED4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="EE4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="EF4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="EG4" s="3" t="s">
         <v>203</v>
       </c>
       <c r="EH4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="EI4" s="3" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="EJ4" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="EK4" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="EL4" s="3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="EM4" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="EN4" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="EO4" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added missing probe data to rq8
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/Research/variables/Variable Definitions RQ8_PH2.xlsx
+++ b/dashboard-ui/src/components/Research/variables/Variable Definitions RQ8_PH2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="217">
   <si>
     <t>Probe</t>
   </si>
@@ -237,6 +237,42 @@
     <t>Urban AF KDMA</t>
   </si>
   <si>
+    <t>Desert Probe1_AF</t>
+  </si>
+  <si>
+    <t>Desert Probe2_AFMF</t>
+  </si>
+  <si>
+    <t>Desert Probe3_AF</t>
+  </si>
+  <si>
+    <t>Desert Probe4_AFMF</t>
+  </si>
+  <si>
+    <t>Desert Probe5_AFMF</t>
+  </si>
+  <si>
+    <t>Desert Probe6_AF</t>
+  </si>
+  <si>
+    <t>Urban Probe1_MF</t>
+  </si>
+  <si>
+    <t>Urban Probe2_MF</t>
+  </si>
+  <si>
+    <t>Urban Probe3_AF</t>
+  </si>
+  <si>
+    <t>Urban Probe4_AF</t>
+  </si>
+  <si>
+    <t>Urban Probe5_MF</t>
+  </si>
+  <si>
+    <t>Urban Probe6_AF</t>
+  </si>
+  <si>
     <t>Desert Personal_safety</t>
   </si>
   <si>
@@ -733,6 +769,9 @@
   </si>
   <si>
     <t>0.0-1.0</t>
+  </si>
+  <si>
+    <t>Patient A or Patient B</t>
   </si>
   <si>
     <t>1 = left the initial zone prior to the all clear, 0 = stayed until safe</t>
@@ -767,7 +806,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -778,6 +817,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -809,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -831,6 +876,12 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,7 +1185,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:EM4"/>
+  <dimension ref="A1:EY4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1151,43 +1202,43 @@
     <col min="9" max="9" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="33" max="33" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="34" max="34" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="35" max="35" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="36" max="36" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="40" max="40" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="41" max="41" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="42" max="42" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="43" max="43" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="44" max="44" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
     <col min="49" max="49" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="50" max="50" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="51" max="51" style="6" width="13.005" customWidth="1" bestFit="1"/>
@@ -1283,9 +1334,21 @@
     <col min="141" max="141" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="142" max="142" style="6" width="13.005" customWidth="1" bestFit="1"/>
     <col min="143" max="143" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="144" max="144" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="145" max="145" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="146" max="146" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="147" max="147" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="148" max="148" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="149" max="149" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="150" max="150" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="151" max="151" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="152" max="152" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="153" max="153" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="154" max="154" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="155" max="155" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="46.5" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="44.25" customFormat="1" s="7">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1319,40 +1382,40 @@
       <c r="K1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="8" t="s">
         <v>40</v>
       </c>
       <c r="X1" s="3" t="s">
@@ -1715,570 +1778,618 @@
       <c r="EM1" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33" customFormat="1" s="7">
+      <c r="EN1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="EO1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="EP1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="EQ1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="ER1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="ES1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="ET1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="EU1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="EV1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="EW1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="EX1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="EY1" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="31.5" customFormat="1" s="7">
       <c r="A2" s="3" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AO2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AQ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AV2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AX2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BC2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BD2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BE2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BF2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BG2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BH2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BI2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BJ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BK2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BL2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BM2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BN2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BO2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BP2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BQ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BR2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BS2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BT2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BU2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BV2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BW2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BX2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BY2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="BZ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CA2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CB2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CC2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CD2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CE2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CF2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CG2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CH2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CI2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CJ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CK2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CL2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CM2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CN2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CO2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CP2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CQ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CR2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CS2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CT2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CU2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CV2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CW2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CX2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CY2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="CZ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DA2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DB2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DC2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DD2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DE2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DF2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DG2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DH2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DI2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DJ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DK2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DL2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DM2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DN2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DO2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DP2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DQ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DR2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DS2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DT2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DU2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DV2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DW2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DX2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DY2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="DZ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EA2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EB2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EC2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="ED2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EE2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EF2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EG2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EH2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EI2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EJ2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EK2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EL2" s="3" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="EM2" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="154.5" customFormat="1" s="7">
+        <v>177</v>
+      </c>
+      <c r="EN2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="EO2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="EP2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="EQ2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="ER2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="ES2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="ET2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="EU2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="EV2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="EW2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="EX2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="EY2" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="146.25" customFormat="1" s="7">
       <c r="A3" s="3" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>176</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
       <c r="X3" s="3" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="AK3" s="3" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="AM3" s="3" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="AO3" s="3" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="AQ3" s="3" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="AR3" s="3" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="AS3" s="3" t="s">
         <v>189</v>
@@ -2290,721 +2401,793 @@
         <v>191</v>
       </c>
       <c r="AV3" s="3" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="AW3" s="3" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="AX3" s="3" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="AY3" s="3" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="AZ3" s="3" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="BA3" s="3" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="BB3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="BC3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="BD3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="BE3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="BF3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="BG3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="BH3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="BI3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="BJ3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="BK3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="BL3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="BM3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="BN3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="BO3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="BP3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="BQ3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="BR3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="BS3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="BT3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="BU3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="BV3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="BW3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="BX3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="BY3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="BZ3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="CA3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="CB3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="CC3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="CD3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="CE3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="CF3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="CG3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="CH3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="CI3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="CJ3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="CK3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="CL3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="CM3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="CN3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="CO3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="CP3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="CQ3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="CR3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="CS3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="CT3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="CU3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="CV3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="CW3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="CX3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="CY3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="CZ3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="DA3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="DB3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="DC3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="DD3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="DE3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="DF3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="DG3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="DH3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="DI3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="DJ3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="DK3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="DL3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="DM3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="DN3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="DO3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="DP3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="DQ3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="DR3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="DS3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="DT3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="DU3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="DV3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="DW3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="DX3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="DY3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="DZ3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="EA3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="EB3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="EC3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="ED3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="EE3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="EF3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="EG3" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="EH3" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="EI3" s="3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="EJ3" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="EK3" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="EL3" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="EM3" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="100.5" customFormat="1" s="7">
+        <v>203</v>
+      </c>
+      <c r="EN3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="EO3" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="EP3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="EQ3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="ER3" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="ES3" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="ET3" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="EU3" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="EV3" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="EW3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="EX3" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="EY3" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="95.25" customFormat="1" s="7">
       <c r="A4" s="3" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>199</v>
+        <v>206</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>207</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="AP4" s="3" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="AQ4" s="3" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="AV4" s="3" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="AW4" s="3" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AX4" s="3" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="AY4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="AZ4" s="3" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BA4" s="3" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="BB4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="BC4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BD4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="BE4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BF4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BG4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="BH4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="BI4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BJ4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="BK4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BL4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BM4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="BN4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="BO4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BP4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="BQ4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BR4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BS4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="BT4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="BU4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BV4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="BW4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BX4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="BY4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="BZ4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="CA4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CB4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="CC4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CD4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CE4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="CF4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="CG4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CH4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="CI4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CJ4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CK4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="CL4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="CM4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CN4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="CO4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CP4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CQ4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="CR4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="CS4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CT4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="CU4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CV4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CW4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="CX4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="CY4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="CZ4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="DA4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DB4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DC4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="DD4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="DE4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DF4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="DG4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DH4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DI4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="DJ4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="DK4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DL4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="DM4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DN4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DO4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="DP4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="DQ4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DR4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="DS4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DT4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DU4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="DV4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="DW4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DX4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="DY4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="DZ4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="EA4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="EB4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="EC4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="ED4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="EE4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="EF4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="EG4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="EH4" s="3" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="EI4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="EJ4" s="3" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="EK4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="EL4" s="3" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="EM4" s="3" t="s">
-        <v>203</v>
+        <v>216</v>
+      </c>
+      <c r="EN4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="EO4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="EP4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="EQ4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="ER4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="ES4" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="ET4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="EU4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="EV4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="EW4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="EX4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="EY4" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>